<commit_message>
schryver data and fixes
Former-commit-id: f5b10110c1383d2e2182a77310770504b0396332
</commit_message>
<xml_diff>
--- a/db/dummydata/schryver/schryver__local_charges.xlsx
+++ b/db/dummydata/schryver/schryver__local_charges.xlsx
@@ -227,10 +227,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -1517,17 +1517,17 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
+      <c r="A43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
       <c r="S43" s="9"/>
     </row>
     <row r="44">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6"/>
+      <c r="A43" s="7"/>
       <c r="C43" s="5" t="s">
         <v>42</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="C2" s="5" t="s">
         <v>25</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>50.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>45.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>90.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>90.0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>190.0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>190.0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>190.0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>30.0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="C20" s="5" t="s">
         <v>40</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="C22" s="5" t="s">
         <v>40</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>14.0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="C24" s="5" t="s">
         <v>40</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>14.0</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="C25" s="5" t="s">
         <v>40</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>14.0</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>50.0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="C28" s="5" t="s">
         <v>41</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="C29" s="5" t="s">
         <v>41</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>190.0</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
@@ -6435,22 +6435,22 @@
       <c r="T30" s="5">
         <v>190.0</v>
       </c>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="8"/>
-      <c r="AD30" s="8"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="8"/>
-      <c r="AG30" s="8"/>
-      <c r="AH30" s="8"/>
-      <c r="AI30" s="8"/>
-      <c r="AJ30" s="8"/>
-      <c r="AK30" s="8"/>
-      <c r="AL30" s="8"/>
-      <c r="AM30" s="8"/>
-    </row>
-    <row r="31">
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AH30" s="6"/>
+      <c r="AI30" s="6"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="6"/>
+      <c r="AL30" s="6"/>
+      <c r="AM30" s="6"/>
+    </row>
+    <row r="31" hidden="1">
       <c r="C31" s="5" t="s">
         <v>41</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>190.0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="C32" s="5" t="s">
         <v>41</v>
       </c>
@@ -6519,22 +6519,22 @@
       <c r="T32" s="5">
         <v>15.0</v>
       </c>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
-      <c r="AD32" s="8"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="8"/>
-      <c r="AI32" s="8"/>
-      <c r="AJ32" s="8"/>
-      <c r="AK32" s="8"/>
-      <c r="AL32" s="8"/>
-      <c r="AM32" s="8"/>
-    </row>
-    <row r="33">
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
+      <c r="AG32" s="6"/>
+      <c r="AH32" s="6"/>
+      <c r="AI32" s="6"/>
+      <c r="AJ32" s="6"/>
+      <c r="AK32" s="6"/>
+      <c r="AL32" s="6"/>
+      <c r="AM32" s="6"/>
+    </row>
+    <row r="33" hidden="1">
       <c r="C33" s="5" t="s">
         <v>41</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="C34" s="5" t="s">
         <v>41</v>
       </c>
@@ -6640,27 +6640,27 @@
       <c r="T35" s="5">
         <v>395.0</v>
       </c>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
-      <c r="AC35" s="8"/>
-      <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
-      <c r="AF35" s="8"/>
-      <c r="AG35" s="8"/>
-      <c r="AH35" s="8"/>
-      <c r="AI35" s="8"/>
-      <c r="AJ35" s="8"/>
-      <c r="AK35" s="8"/>
-      <c r="AL35" s="8"/>
-      <c r="AM35" s="8"/>
-    </row>
-    <row r="36">
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="6"/>
+      <c r="AG35" s="6"/>
+      <c r="AH35" s="6"/>
+      <c r="AI35" s="6"/>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="6"/>
+      <c r="AL35" s="6"/>
+      <c r="AM35" s="6"/>
+    </row>
+    <row r="36" hidden="1">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
@@ -6696,27 +6696,27 @@
       <c r="T36" s="5">
         <v>790.0</v>
       </c>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
-      <c r="AC36" s="8"/>
-      <c r="AD36" s="8"/>
-      <c r="AE36" s="8"/>
-      <c r="AF36" s="8"/>
-      <c r="AG36" s="8"/>
-      <c r="AH36" s="8"/>
-      <c r="AI36" s="8"/>
-      <c r="AJ36" s="8"/>
-      <c r="AK36" s="8"/>
-      <c r="AL36" s="8"/>
-      <c r="AM36" s="8"/>
-    </row>
-    <row r="37">
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="6"/>
+      <c r="AE36" s="6"/>
+      <c r="AF36" s="6"/>
+      <c r="AG36" s="6"/>
+      <c r="AH36" s="6"/>
+      <c r="AI36" s="6"/>
+      <c r="AJ36" s="6"/>
+      <c r="AK36" s="6"/>
+      <c r="AL36" s="6"/>
+      <c r="AM36" s="6"/>
+    </row>
+    <row r="37" hidden="1">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="5" t="s">
@@ -6790,7 +6790,7 @@
         <v>42.0</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="5" t="s">
@@ -6827,7 +6827,7 @@
         <v>84.0</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="5" t="s">
@@ -6899,7 +6899,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="C42" s="5" t="s">
         <v>42</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="C43" s="5" t="s">
         <v>42</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>55.0</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="C45" s="5" t="s">
         <v>42</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="C46" s="5" t="s">
         <v>42</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="C48" s="5" t="s">
         <v>25</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="C49" s="5" t="s">
         <v>25</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="C51" s="5" t="s">
         <v>25</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1">
       <c r="C52" s="5" t="s">
         <v>25</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>55.0</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="C54" s="5" t="s">
         <v>25</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="C55" s="5" t="s">
         <v>25</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>90.0</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="C57" s="5" t="s">
         <v>47</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="C58" s="5" t="s">
         <v>47</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="C60" s="5" t="s">
         <v>47</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="C61" s="5" t="s">
         <v>47</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c r="C63" s="5" t="s">
         <v>47</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>120.0</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="C64" s="5" t="s">
         <v>47</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>205.0</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="C66" s="5" t="s">
         <v>48</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>410.0</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="C67" s="5" t="s">
         <v>48</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c r="C69" s="5" t="s">
         <v>48</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c r="C70" s="5" t="s">
         <v>48</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="C71" s="5" t="s">
         <v>42</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>395.0</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c r="C72" s="5" t="s">
         <v>42</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>790.0</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="C73" s="5" t="s">
         <v>42</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>790.0</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="C74" s="5" t="s">
         <v>42</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>42.0</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="C75" s="5" t="s">
         <v>42</v>
       </c>
@@ -8089,7 +8089,7 @@
         <v>84.0</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="C76" s="5" t="s">
         <v>42</v>
       </c>
@@ -8124,7 +8124,7 @@
         <v>84.0</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="C77" s="5" t="s">
         <v>42</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="C78" s="5" t="s">
         <v>42</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="C79" s="5" t="s">
         <v>42</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="C80" s="5" t="s">
         <v>42</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>55.0</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c r="C81" s="5" t="s">
         <v>42</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c r="C82" s="5" t="s">
         <v>42</v>
       </c>
@@ -8334,7 +8334,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c r="C83" s="5" t="s">
         <v>25</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c r="C84" s="5" t="s">
         <v>25</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="C85" s="5" t="s">
         <v>25</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="C86" s="5" t="s">
         <v>25</v>
       </c>
@@ -8474,7 +8474,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="C87" s="5" t="s">
         <v>25</v>
       </c>
@@ -8509,7 +8509,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="C88" s="5" t="s">
         <v>25</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="C89" s="5" t="s">
         <v>25</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>55.0</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="C90" s="5" t="s">
         <v>25</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c r="C91" s="5" t="s">
         <v>25</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>110.0</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="C92" s="5" t="s">
         <v>47</v>
       </c>
@@ -8684,7 +8684,7 @@
         <v>90.0</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="C93" s="5" t="s">
         <v>47</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="C94" s="5" t="s">
         <v>47</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c r="C95" s="5" t="s">
         <v>47</v>
       </c>
@@ -8789,7 +8789,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="C96" s="5" t="s">
         <v>47</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="C97" s="5" t="s">
         <v>47</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="C98" s="5" t="s">
         <v>47</v>
       </c>
@@ -8894,7 +8894,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="C99" s="5" t="s">
         <v>47</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>120.0</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="C100" s="5" t="s">
         <v>47</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>120.0</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="C101" s="5" t="s">
         <v>48</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>205.0</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1">
       <c r="C102" s="5" t="s">
         <v>48</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>410.0</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1">
       <c r="C103" s="5" t="s">
         <v>48</v>
       </c>
@@ -9069,7 +9069,7 @@
         <v>410.0</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1">
       <c r="C104" s="5" t="s">
         <v>48</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" hidden="1">
       <c r="C105" s="5" t="s">
         <v>48</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>35.0</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="1">
       <c r="C106" s="5" t="s">
         <v>48</v>
       </c>
@@ -9175,7 +9175,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$V$106"/>
+  <autoFilter ref="$A$1:$V$106">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="fcl_20"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Altamira"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>